<commit_message>
correcting extreme values in counties, municipalities
</commit_message>
<xml_diff>
--- a/data/_dictionary_acfrID_censusGEOID.xlsx
+++ b/data/_dictionary_acfrID_censusGEOID.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tn/Desktop/REASON/acfrs_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BBFE98-1EEA-D147-87D3-3EBD4F9C358B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCBB1B6-55E6-734D-9E70-59F3192D022D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="5860" windowWidth="29080" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="6100" windowWidth="29080" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="76">
   <si>
     <t>state.abb</t>
   </si>
@@ -143,13 +156,118 @@
   </si>
   <si>
     <t>mount morris charter township</t>
+  </si>
+  <si>
+    <t>kingston</t>
+  </si>
+  <si>
+    <t>northampton township</t>
+  </si>
+  <si>
+    <t>4254688</t>
+  </si>
+  <si>
+    <t>5508225</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bloomer </t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>webster city</t>
+  </si>
+  <si>
+    <t>1983145</t>
+  </si>
+  <si>
+    <t>0660620</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>richmond</t>
+  </si>
+  <si>
+    <t>5531000</t>
+  </si>
+  <si>
+    <t>green bay</t>
+  </si>
+  <si>
+    <t>0827425</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>melbourne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PA </t>
+  </si>
+  <si>
+    <t>bradford</t>
+  </si>
+  <si>
+    <t>susquehanna township</t>
+  </si>
+  <si>
+    <t>oshkosh</t>
+  </si>
+  <si>
+    <t>greenfield</t>
+  </si>
+  <si>
+    <t>caledonia</t>
+  </si>
+  <si>
+    <t>lawrence</t>
+  </si>
+  <si>
+    <t>howard</t>
+  </si>
+  <si>
+    <t>butler</t>
+  </si>
+  <si>
+    <t>manitowoc</t>
+  </si>
+  <si>
+    <t>newtown</t>
+  </si>
+  <si>
+    <t>franklin</t>
+  </si>
+  <si>
+    <t>exeter township</t>
+  </si>
+  <si>
+    <t>millcreek township</t>
+  </si>
+  <si>
+    <t>middletown</t>
+  </si>
+  <si>
+    <t>watertown</t>
+  </si>
+  <si>
+    <t>oswego</t>
+  </si>
+  <si>
+    <t>binghamton</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,13 +306,38 @@
       <name val="Lucida Grande"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -209,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -224,6 +367,10 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,16 +675,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" customWidth="1"/>
     <col min="3" max="3" width="16.5" customWidth="1"/>
     <col min="4" max="4" width="14.83203125" style="9" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
@@ -946,6 +1093,350 @@
         <v>2655980</v>
       </c>
     </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="10">
+        <v>36064</v>
+      </c>
+      <c r="D30" s="3">
+        <v>3639727</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31">
+        <v>1266152</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32">
+        <v>131132</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33">
+        <v>71110</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34">
+        <v>1265296</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35">
+        <v>39880</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <v>138430</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="10">
+        <v>92009</v>
+      </c>
+      <c r="D37" s="3">
+        <v>1243975</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="12">
+        <v>122977</v>
+      </c>
+      <c r="D38" s="3">
+        <v>4208040</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39">
+        <v>1266159</v>
+      </c>
+      <c r="D39" s="3">
+        <v>4275528</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40">
+        <v>39904</v>
+      </c>
+      <c r="D40" s="3">
+        <v>5560500</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="12">
+        <v>131380</v>
+      </c>
+      <c r="D41" s="3">
+        <v>5531175</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42">
+        <v>1036134</v>
+      </c>
+      <c r="D42" s="3">
+        <v>5511950</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43">
+        <v>131695</v>
+      </c>
+      <c r="D43" s="3">
+        <v>5542900</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" s="10">
+        <v>1036138</v>
+      </c>
+      <c r="D44" s="3">
+        <v>5535950</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45">
+        <v>131574</v>
+      </c>
+      <c r="D45" s="3">
+        <v>5511475</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>67</v>
+      </c>
+      <c r="C46">
+        <v>89528</v>
+      </c>
+      <c r="D46" s="11">
+        <v>5548500</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C47" s="13">
+        <v>68300</v>
+      </c>
+      <c r="D47" s="11">
+        <v>952980</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C48" s="13">
+        <v>131370</v>
+      </c>
+      <c r="D48" s="11">
+        <v>5527300</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49" s="13">
+        <v>127137</v>
+      </c>
+      <c r="D49" s="11">
+        <v>4224384</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>23</v>
+      </c>
+      <c r="B50" t="s">
+        <v>71</v>
+      </c>
+      <c r="C50">
+        <v>127357</v>
+      </c>
+      <c r="D50" s="11">
+        <v>4249548</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>27</v>
+      </c>
+      <c r="B51" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51">
+        <v>43361</v>
+      </c>
+      <c r="D51" s="11">
+        <v>3647042</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>27</v>
+      </c>
+      <c r="B52" t="s">
+        <v>73</v>
+      </c>
+      <c r="C52">
+        <v>36034</v>
+      </c>
+      <c r="D52" s="11">
+        <v>3678608</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" t="s">
+        <v>74</v>
+      </c>
+      <c r="C53">
+        <v>1035911</v>
+      </c>
+      <c r="D53" s="11">
+        <v>3655574</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54" t="s">
+        <v>75</v>
+      </c>
+      <c r="C54">
+        <v>1035909</v>
+      </c>
+      <c r="D54" s="11">
+        <v>3606607</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>